<commit_message>
Entrega de guión 01 matemáticas 03
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado04/guion01/SolicitudGrafica_MA_04_01_CO_REC30.xlsx
+++ b/fuentes/contenidos/grado04/guion01/SolicitudGrafica_MA_04_01_CO_REC30.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Copia\JOHANNA\Documents\Documents\Matematicas\fuentes\contenidos\grado04\guion01\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23760" windowHeight="14560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Solicitud gráfica" sheetId="1" r:id="rId1"/>
     <sheet name="Ayuda" sheetId="2" r:id="rId2"/>
     <sheet name="Definición técnica de imagenes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -991,11 +986,11 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1004,7 +999,7 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1012,17 +1007,17 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -1032,7 +1027,7 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -1040,12 +1035,12 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1054,18 +1049,18 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1095,11 +1090,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color auto="1"/>
@@ -1109,10 +1104,10 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color auto="1"/>
@@ -1122,7 +1117,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
         <color auto="1"/>
@@ -1196,16 +1191,16 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1213,23 +1208,23 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2076,15 +2071,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>25400</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1038225</xdr:colOff>
+          <xdr:colOff>1041400</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>238125</xdr:rowOff>
+          <xdr:rowOff>241300</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2097,7 +2092,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2105,20 +2100,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2131,15 +2112,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1047750</xdr:colOff>
+          <xdr:colOff>1054100</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>866775</xdr:colOff>
+          <xdr:colOff>863600</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>238125</xdr:rowOff>
+          <xdr:rowOff>241300</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2152,7 +2133,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2160,20 +2141,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2186,15 +2153,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>25400</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>238125</xdr:rowOff>
+          <xdr:rowOff>241300</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2207,7 +2174,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2215,20 +2182,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2243,13 +2196,13 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>485775</xdr:rowOff>
+          <xdr:rowOff>482600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1019175</xdr:colOff>
+          <xdr:colOff>1016000</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>714375</xdr:rowOff>
+          <xdr:rowOff>711200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2262,7 +2215,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2270,20 +2223,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2296,15 +2235,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1019175</xdr:colOff>
+          <xdr:colOff>1016000</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>485775</xdr:rowOff>
+          <xdr:rowOff>482600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>828675</xdr:colOff>
+          <xdr:colOff>825500</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>714375</xdr:rowOff>
+          <xdr:rowOff>711200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2317,7 +2256,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2325,20 +2264,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2351,15 +2276,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>485775</xdr:rowOff>
+          <xdr:rowOff>482600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>838200</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>714375</xdr:rowOff>
+          <xdr:rowOff>711200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2372,7 +2297,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2380,20 +2305,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2406,15 +2317,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>485775</xdr:rowOff>
+          <xdr:rowOff>482600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
           <xdr:colOff>838200</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>714375</xdr:rowOff>
+          <xdr:rowOff>711200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2427,7 +2338,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2435,20 +2346,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2781,32 +2678,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja1"/>
+  <sheetPr codeName="Hoja1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.875" style="57" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" style="57" customWidth="1"/>
     <col min="2" max="2" width="21" style="57" customWidth="1"/>
-    <col min="3" max="3" width="21.25" style="57" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" style="57" customWidth="1"/>
     <col min="4" max="4" width="18.5" style="57" customWidth="1"/>
-    <col min="5" max="5" width="13.125" style="57" customWidth="1"/>
-    <col min="6" max="6" width="28.25" style="57" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" style="57" customWidth="1"/>
+    <col min="6" max="6" width="28.1640625" style="57" customWidth="1"/>
     <col min="7" max="7" width="20.5" style="57" customWidth="1"/>
-    <col min="8" max="8" width="28.625" style="57" customWidth="1"/>
+    <col min="8" max="8" width="28.6640625" style="57" customWidth="1"/>
     <col min="9" max="9" width="20.5" style="57" customWidth="1"/>
-    <col min="10" max="10" width="34.875" style="60" customWidth="1"/>
+    <col min="10" max="10" width="34.83203125" style="60" customWidth="1"/>
     <col min="11" max="11" width="56.5" style="60" customWidth="1"/>
-    <col min="12" max="12" width="20.375" style="57" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" style="57" customWidth="1"/>
     <col min="13" max="13" width="14.5" style="57" customWidth="1"/>
-    <col min="14" max="16384" width="10.875" style="57"/>
+    <col min="14" max="16384" width="10.83203125" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="16.5" thickBot="1">
       <c r="A1" s="56"/>
       <c r="B1" s="56"/>
       <c r="C1" s="56"/>
@@ -2818,7 +2715,7 @@
       <c r="J1" s="24"/>
       <c r="K1" s="24"/>
     </row>
-    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="15.75">
       <c r="A2" s="56"/>
       <c r="B2" s="59" t="s">
         <v>0</v>
@@ -2835,7 +2732,7 @@
       <c r="I2" s="58"/>
       <c r="J2" s="24"/>
     </row>
-    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="15.75">
       <c r="A3" s="56"/>
       <c r="B3" s="61" t="s">
         <v>9</v>
@@ -2850,7 +2747,7 @@
       <c r="I3" s="58"/>
       <c r="J3" s="24"/>
     </row>
-    <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="15.75">
       <c r="A4" s="56"/>
       <c r="B4" s="61" t="s">
         <v>55</v>
@@ -2871,7 +2768,7 @@
       <c r="J4" s="24"/>
       <c r="K4" s="24"/>
     </row>
-    <row r="5" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="16.5" thickBot="1">
       <c r="A5" s="56"/>
       <c r="B5" s="64" t="s">
         <v>2</v>
@@ -2893,7 +2790,7 @@
       <c r="J5" s="24"/>
       <c r="K5" s="24"/>
     </row>
-    <row r="6" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="16.5" thickBot="1">
       <c r="A6" s="56"/>
       <c r="B6" s="56"/>
       <c r="C6" s="56"/>
@@ -2906,7 +2803,7 @@
       <c r="J6" s="24"/>
       <c r="K6" s="24"/>
     </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="15" customHeight="1">
       <c r="A7" s="56"/>
       <c r="B7" s="17" t="s">
         <v>41</v>
@@ -2924,7 +2821,7 @@
       <c r="J7" s="24"/>
       <c r="K7" s="24"/>
     </row>
-    <row r="8" spans="1:16" s="73" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" s="73" customFormat="1" ht="16.5" thickBot="1">
       <c r="A8" s="69"/>
       <c r="B8" s="69"/>
       <c r="C8" s="69"/>
@@ -2944,7 +2841,7 @@
       <c r="O8" s="57"/>
       <c r="P8" s="57"/>
     </row>
-    <row r="9" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="26.25" thickBot="1">
       <c r="A9" s="15" t="s">
         <v>3</v>
       </c>
@@ -2979,7 +2876,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="72" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="72" customFormat="1" ht="40.5">
       <c r="A10" s="2" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),"IMG01","")</f>
         <v>IMG01</v>
@@ -3018,7 +2915,7 @@
       </c>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="1:16" s="72" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" s="72" customFormat="1" ht="40.5">
       <c r="A11" s="2" t="s">
         <v>153</v>
       </c>
@@ -3056,7 +2953,7 @@
       </c>
       <c r="K11" s="3"/>
     </row>
-    <row r="12" spans="1:16" s="72" customFormat="1" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="72" customFormat="1" ht="131.25" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>156</v>
       </c>
@@ -3094,7 +2991,7 @@
       </c>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="1:16" s="72" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="72" customFormat="1" ht="40.5">
       <c r="A13" s="2" t="str">
         <f t="shared" ref="A13:A30" si="3">IF(OR(B13&lt;&gt;"",J13&lt;&gt;""),CONCATENATE(LEFT(A12,3),IF(MID(A12,4,2)+1&lt;10,CONCATENATE("0",MID(A12,4,2)+1))),"")</f>
         <v>IMG04</v>
@@ -3133,7 +3030,7 @@
       </c>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:16" s="72" customFormat="1" ht="124.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="72" customFormat="1" ht="125" customHeight="1">
       <c r="A14" s="2" t="str">
         <f t="shared" si="3"/>
         <v>IMG05</v>
@@ -3172,7 +3069,7 @@
       </c>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="1:16" s="72" customFormat="1" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="72" customFormat="1" ht="162.75" customHeight="1">
       <c r="A15" s="54" t="s">
         <v>160</v>
       </c>
@@ -3210,7 +3107,7 @@
       </c>
       <c r="K15" s="13"/>
     </row>
-    <row r="16" spans="1:16" s="72" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" s="72" customFormat="1" ht="53.25" customHeight="1">
       <c r="A16" s="2" t="str">
         <f t="shared" si="3"/>
         <v>IMG07</v>
@@ -3249,7 +3146,7 @@
       </c>
       <c r="K16" s="74"/>
     </row>
-    <row r="17" spans="1:11" s="72" customFormat="1" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="72" customFormat="1" ht="160.5" customHeight="1">
       <c r="A17" s="54" t="s">
         <v>163</v>
       </c>
@@ -3287,7 +3184,7 @@
       </c>
       <c r="K17" s="13"/>
     </row>
-    <row r="18" spans="1:11" s="72" customFormat="1" ht="192.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="72" customFormat="1" ht="192.75" customHeight="1">
       <c r="A18" s="54" t="s">
         <v>165</v>
       </c>
@@ -3325,7 +3222,7 @@
       </c>
       <c r="K18" s="13"/>
     </row>
-    <row r="19" spans="1:11" s="72" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="72" customFormat="1" ht="27" customHeight="1">
       <c r="A19" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3356,7 +3253,7 @@
       <c r="J19" s="13"/>
       <c r="K19" s="74"/>
     </row>
-    <row r="20" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="72" customFormat="1" ht="15">
       <c r="A20" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3387,7 +3284,7 @@
       <c r="J20" s="4"/>
       <c r="K20" s="13"/>
     </row>
-    <row r="21" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="72" customFormat="1" ht="15">
       <c r="A21" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3418,7 +3315,7 @@
       <c r="J21" s="13"/>
       <c r="K21" s="13"/>
     </row>
-    <row r="22" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="72" customFormat="1" ht="15">
       <c r="A22" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3449,7 +3346,7 @@
       <c r="J22" s="3"/>
       <c r="K22" s="4"/>
     </row>
-    <row r="23" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="72" customFormat="1" ht="15">
       <c r="A23" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3477,7 +3374,7 @@
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="72" customFormat="1" ht="15">
       <c r="A24" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3505,7 +3402,7 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
     </row>
-    <row r="25" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="72" customFormat="1" ht="15">
       <c r="A25" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3533,7 +3430,7 @@
       <c r="J25" s="3"/>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="72" customFormat="1" ht="15">
       <c r="A26" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3561,7 +3458,7 @@
       <c r="J26" s="3"/>
       <c r="K26" s="4"/>
     </row>
-    <row r="27" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="72" customFormat="1" ht="15">
       <c r="A27" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3589,7 +3486,7 @@
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
     </row>
-    <row r="28" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="72" customFormat="1" ht="15">
       <c r="A28" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3617,7 +3514,7 @@
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
     </row>
-    <row r="29" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="72" customFormat="1" ht="15">
       <c r="A29" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3645,7 +3542,7 @@
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
     </row>
-    <row r="30" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" s="72" customFormat="1" ht="15">
       <c r="A30" s="2" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3673,7 +3570,7 @@
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
     </row>
-    <row r="31" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" s="72" customFormat="1">
       <c r="A31" s="2"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
@@ -3698,7 +3595,7 @@
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
     </row>
-    <row r="32" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" s="72" customFormat="1">
       <c r="A32" s="2"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
@@ -3723,7 +3620,7 @@
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
     </row>
-    <row r="33" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" s="72" customFormat="1">
       <c r="A33" s="2"/>
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
@@ -3748,7 +3645,7 @@
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
     </row>
-    <row r="34" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" s="72" customFormat="1">
       <c r="A34" s="2"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
@@ -3773,7 +3670,7 @@
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
     </row>
-    <row r="35" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" s="72" customFormat="1">
       <c r="A35" s="2"/>
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
@@ -3798,7 +3695,7 @@
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
     </row>
-    <row r="36" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" s="72" customFormat="1">
       <c r="A36" s="2"/>
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
@@ -3823,7 +3720,7 @@
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
     </row>
-    <row r="37" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" s="72" customFormat="1">
       <c r="A37" s="2"/>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
@@ -3848,7 +3745,7 @@
       <c r="J37" s="5"/>
       <c r="K37" s="3"/>
     </row>
-    <row r="38" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" s="72" customFormat="1">
       <c r="A38" s="2"/>
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
@@ -3873,7 +3770,7 @@
       <c r="J38" s="5"/>
       <c r="K38" s="3"/>
     </row>
-    <row r="39" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" s="72" customFormat="1">
       <c r="A39" s="2"/>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
@@ -3898,7 +3795,7 @@
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
     </row>
-    <row r="40" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" s="72" customFormat="1">
       <c r="A40" s="2"/>
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
@@ -3923,7 +3820,7 @@
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
     </row>
-    <row r="41" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" s="72" customFormat="1">
       <c r="A41" s="2"/>
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
@@ -3948,7 +3845,7 @@
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
     </row>
-    <row r="42" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" s="72" customFormat="1">
       <c r="A42" s="2"/>
       <c r="B42" s="9"/>
       <c r="C42" s="9"/>
@@ -3973,7 +3870,7 @@
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
     </row>
-    <row r="43" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" s="72" customFormat="1">
       <c r="A43" s="2"/>
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
@@ -3998,7 +3895,7 @@
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
     </row>
-    <row r="44" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" s="72" customFormat="1">
       <c r="A44" s="2"/>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
@@ -4023,7 +3920,7 @@
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
     </row>
-    <row r="45" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" s="72" customFormat="1">
       <c r="A45" s="2"/>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
@@ -4048,7 +3945,7 @@
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
     </row>
-    <row r="46" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" s="72" customFormat="1">
       <c r="A46" s="2"/>
       <c r="B46" s="9"/>
       <c r="C46" s="9"/>
@@ -4073,7 +3970,7 @@
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
     </row>
-    <row r="47" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" s="72" customFormat="1">
       <c r="A47" s="2"/>
       <c r="B47" s="9"/>
       <c r="C47" s="9"/>
@@ -4098,7 +3995,7 @@
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
     </row>
-    <row r="48" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" s="72" customFormat="1">
       <c r="A48" s="2"/>
       <c r="B48" s="9"/>
       <c r="C48" s="9"/>
@@ -4123,7 +4020,7 @@
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
     </row>
-    <row r="49" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" s="72" customFormat="1">
       <c r="A49" s="2"/>
       <c r="B49" s="9"/>
       <c r="C49" s="9"/>
@@ -4148,7 +4045,7 @@
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
     </row>
-    <row r="50" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" s="72" customFormat="1">
       <c r="A50" s="2"/>
       <c r="B50" s="9"/>
       <c r="C50" s="9"/>
@@ -4173,7 +4070,7 @@
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
     </row>
-    <row r="51" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" s="72" customFormat="1">
       <c r="A51" s="2"/>
       <c r="B51" s="9"/>
       <c r="C51" s="9"/>
@@ -4198,7 +4095,7 @@
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
     </row>
-    <row r="52" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" s="72" customFormat="1">
       <c r="A52" s="2"/>
       <c r="B52" s="9"/>
       <c r="C52" s="9"/>
@@ -4223,7 +4120,7 @@
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
     </row>
-    <row r="53" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" s="72" customFormat="1">
       <c r="A53" s="2"/>
       <c r="B53" s="9"/>
       <c r="C53" s="9"/>
@@ -4248,7 +4145,7 @@
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
     </row>
-    <row r="54" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" s="72" customFormat="1">
       <c r="A54" s="2"/>
       <c r="B54" s="9"/>
       <c r="C54" s="9"/>
@@ -4273,7 +4170,7 @@
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
     </row>
-    <row r="55" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" s="72" customFormat="1">
       <c r="A55" s="2"/>
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
@@ -4298,7 +4195,7 @@
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
     </row>
-    <row r="56" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" s="72" customFormat="1">
       <c r="A56" s="2"/>
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
@@ -4323,7 +4220,7 @@
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
     </row>
-    <row r="57" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" s="72" customFormat="1">
       <c r="A57" s="2"/>
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
@@ -4348,7 +4245,7 @@
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
     </row>
-    <row r="58" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" s="72" customFormat="1">
       <c r="A58" s="2"/>
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
@@ -4373,7 +4270,7 @@
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
     </row>
-    <row r="59" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" s="72" customFormat="1">
       <c r="A59" s="2"/>
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
@@ -4398,7 +4295,7 @@
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
     </row>
-    <row r="60" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" s="72" customFormat="1">
       <c r="A60" s="2"/>
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
@@ -4423,7 +4320,7 @@
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
     </row>
-    <row r="61" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" s="72" customFormat="1">
       <c r="A61" s="2"/>
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
@@ -4448,7 +4345,7 @@
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
     </row>
-    <row r="62" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" s="72" customFormat="1">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -4473,7 +4370,7 @@
       <c r="J62" s="3"/>
       <c r="K62" s="3"/>
     </row>
-    <row r="63" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" s="72" customFormat="1">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -4498,7 +4395,7 @@
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
     </row>
-    <row r="64" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" s="72" customFormat="1">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -4523,7 +4420,7 @@
       <c r="J64" s="3"/>
       <c r="K64" s="3"/>
     </row>
-    <row r="65" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" s="72" customFormat="1">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -4548,7 +4445,7 @@
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
     </row>
-    <row r="66" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" s="72" customFormat="1">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -4573,7 +4470,7 @@
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
     </row>
-    <row r="67" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" s="72" customFormat="1">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -4598,7 +4495,7 @@
       <c r="J67" s="3"/>
       <c r="K67" s="3"/>
     </row>
-    <row r="68" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" s="72" customFormat="1">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -4623,7 +4520,7 @@
       <c r="J68" s="3"/>
       <c r="K68" s="3"/>
     </row>
-    <row r="69" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" s="72" customFormat="1">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -4648,7 +4545,7 @@
       <c r="J69" s="3"/>
       <c r="K69" s="3"/>
     </row>
-    <row r="70" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" s="72" customFormat="1">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -4673,7 +4570,7 @@
       <c r="J70" s="3"/>
       <c r="K70" s="3"/>
     </row>
-    <row r="71" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" s="72" customFormat="1">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -4698,7 +4595,7 @@
       <c r="J71" s="3"/>
       <c r="K71" s="3"/>
     </row>
-    <row r="72" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" s="72" customFormat="1">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -4723,7 +4620,7 @@
       <c r="J72" s="3"/>
       <c r="K72" s="3"/>
     </row>
-    <row r="73" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" s="72" customFormat="1">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -4748,7 +4645,7 @@
       <c r="J73" s="3"/>
       <c r="K73" s="3"/>
     </row>
-    <row r="74" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" s="72" customFormat="1">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -4773,7 +4670,7 @@
       <c r="J74" s="3"/>
       <c r="K74" s="3"/>
     </row>
-    <row r="75" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" s="72" customFormat="1">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -4798,7 +4695,7 @@
       <c r="J75" s="3"/>
       <c r="K75" s="3"/>
     </row>
-    <row r="76" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" s="72" customFormat="1">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -4823,7 +4720,7 @@
       <c r="J76" s="3"/>
       <c r="K76" s="3"/>
     </row>
-    <row r="77" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" s="72" customFormat="1">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -4848,7 +4745,7 @@
       <c r="J77" s="3"/>
       <c r="K77" s="3"/>
     </row>
-    <row r="78" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" s="72" customFormat="1">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -4873,7 +4770,7 @@
       <c r="J78" s="3"/>
       <c r="K78" s="3"/>
     </row>
-    <row r="79" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" s="72" customFormat="1">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -4898,7 +4795,7 @@
       <c r="J79" s="3"/>
       <c r="K79" s="3"/>
     </row>
-    <row r="80" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" s="72" customFormat="1">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -4923,7 +4820,7 @@
       <c r="J80" s="3"/>
       <c r="K80" s="3"/>
     </row>
-    <row r="81" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" s="72" customFormat="1">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -4948,7 +4845,7 @@
       <c r="J81" s="3"/>
       <c r="K81" s="3"/>
     </row>
-    <row r="82" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" s="72" customFormat="1">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -4973,7 +4870,7 @@
       <c r="J82" s="3"/>
       <c r="K82" s="3"/>
     </row>
-    <row r="83" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" s="72" customFormat="1">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -4998,7 +4895,7 @@
       <c r="J83" s="3"/>
       <c r="K83" s="3"/>
     </row>
-    <row r="84" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" s="72" customFormat="1">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -5023,7 +4920,7 @@
       <c r="J84" s="3"/>
       <c r="K84" s="3"/>
     </row>
-    <row r="85" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" s="72" customFormat="1">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -5048,7 +4945,7 @@
       <c r="J85" s="3"/>
       <c r="K85" s="3"/>
     </row>
-    <row r="86" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" s="72" customFormat="1">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -5073,7 +4970,7 @@
       <c r="J86" s="3"/>
       <c r="K86" s="3"/>
     </row>
-    <row r="87" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" s="72" customFormat="1">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -5098,7 +4995,7 @@
       <c r="J87" s="3"/>
       <c r="K87" s="3"/>
     </row>
-    <row r="88" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" s="72" customFormat="1">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -5123,7 +5020,7 @@
       <c r="J88" s="3"/>
       <c r="K88" s="3"/>
     </row>
-    <row r="89" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" s="72" customFormat="1">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -5148,7 +5045,7 @@
       <c r="J89" s="3"/>
       <c r="K89" s="3"/>
     </row>
-    <row r="90" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" s="72" customFormat="1">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -5173,7 +5070,7 @@
       <c r="J90" s="3"/>
       <c r="K90" s="3"/>
     </row>
-    <row r="91" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" s="72" customFormat="1">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -5198,7 +5095,7 @@
       <c r="J91" s="3"/>
       <c r="K91" s="3"/>
     </row>
-    <row r="92" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" s="72" customFormat="1">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -5223,7 +5120,7 @@
       <c r="J92" s="3"/>
       <c r="K92" s="3"/>
     </row>
-    <row r="93" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" s="72" customFormat="1">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -5248,7 +5145,7 @@
       <c r="J93" s="3"/>
       <c r="K93" s="3"/>
     </row>
-    <row r="94" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" s="72" customFormat="1">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -5273,7 +5170,7 @@
       <c r="J94" s="3"/>
       <c r="K94" s="3"/>
     </row>
-    <row r="95" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" s="72" customFormat="1">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -5298,7 +5195,7 @@
       <c r="J95" s="3"/>
       <c r="K95" s="3"/>
     </row>
-    <row r="96" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" s="72" customFormat="1">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -5323,7 +5220,7 @@
       <c r="J96" s="3"/>
       <c r="K96" s="3"/>
     </row>
-    <row r="97" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" s="72" customFormat="1">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -5348,7 +5245,7 @@
       <c r="J97" s="3"/>
       <c r="K97" s="3"/>
     </row>
-    <row r="98" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" s="72" customFormat="1">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -5373,7 +5270,7 @@
       <c r="J98" s="3"/>
       <c r="K98" s="3"/>
     </row>
-    <row r="99" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" s="72" customFormat="1">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -5398,7 +5295,7 @@
       <c r="J99" s="3"/>
       <c r="K99" s="3"/>
     </row>
-    <row r="100" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" s="72" customFormat="1">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -5423,7 +5320,7 @@
       <c r="J100" s="3"/>
       <c r="K100" s="3"/>
     </row>
-    <row r="101" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" s="72" customFormat="1">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -5448,7 +5345,7 @@
       <c r="J101" s="3"/>
       <c r="K101" s="3"/>
     </row>
-    <row r="102" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" s="72" customFormat="1">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -5473,7 +5370,7 @@
       <c r="J102" s="3"/>
       <c r="K102" s="3"/>
     </row>
-    <row r="103" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" s="72" customFormat="1">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -5498,7 +5395,7 @@
       <c r="J103" s="3"/>
       <c r="K103" s="3"/>
     </row>
-    <row r="104" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" s="72" customFormat="1">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -5523,7 +5420,7 @@
       <c r="J104" s="3"/>
       <c r="K104" s="3"/>
     </row>
-    <row r="105" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" s="72" customFormat="1">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -5548,7 +5445,7 @@
       <c r="J105" s="3"/>
       <c r="K105" s="3"/>
     </row>
-    <row r="106" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" s="72" customFormat="1">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -5573,7 +5470,7 @@
       <c r="J106" s="3"/>
       <c r="K106" s="3"/>
     </row>
-    <row r="107" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" s="72" customFormat="1">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -5598,7 +5495,7 @@
       <c r="J107" s="3"/>
       <c r="K107" s="3"/>
     </row>
-    <row r="108" spans="1:11" s="72" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" s="72" customFormat="1">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -5671,8 +5568,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5683,25 +5579,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja2"/>
+  <sheetPr codeName="Hoja2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="72.25" style="16" customWidth="1"/>
-    <col min="2" max="2" width="11" style="16"/>
-    <col min="3" max="3" width="13.875" style="16" customWidth="1"/>
-    <col min="4" max="4" width="11.375" style="16" customWidth="1"/>
-    <col min="5" max="7" width="11" style="16"/>
+    <col min="1" max="1" width="72.1640625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="16"/>
+    <col min="3" max="3" width="13.83203125" style="16" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="16" customWidth="1"/>
+    <col min="5" max="7" width="10.83203125" style="16"/>
     <col min="8" max="11" width="11" style="16" hidden="1" customWidth="1"/>
-    <col min="12" max="16384" width="11" style="16"/>
+    <col min="12" max="16384" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="16.5" thickBot="1">
       <c r="A1" s="91" t="s">
         <v>39</v>
       </c>
@@ -5711,7 +5607,7 @@
       <c r="E1" s="92"/>
       <c r="F1" s="93"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="23" t="s">
         <v>43</v>
       </c>
@@ -5723,7 +5619,7 @@
       <c r="E2" s="96"/>
       <c r="F2" s="25"/>
     </row>
-    <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="63">
       <c r="A3" s="26" t="s">
         <v>44</v>
       </c>
@@ -5747,7 +5643,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="31.5">
       <c r="A4" s="23" t="s">
         <v>45</v>
       </c>
@@ -5775,7 +5671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="79.5" thickBot="1">
       <c r="A5" s="26" t="s">
         <v>46</v>
       </c>
@@ -5802,7 +5698,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="32.25" thickBot="1">
       <c r="A6" s="23" t="s">
         <v>11</v>
       </c>
@@ -5824,7 +5720,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="48" thickBot="1">
       <c r="A7" s="26" t="s">
         <v>12</v>
       </c>
@@ -5851,7 +5747,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="47.25">
       <c r="A8" s="26" t="s">
         <v>54</v>
       </c>
@@ -5870,7 +5766,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="47.25">
       <c r="A9" s="26" t="s">
         <v>13</v>
       </c>
@@ -5889,7 +5785,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="32.25" thickBot="1">
       <c r="A10" s="27" t="s">
         <v>37</v>
       </c>
@@ -5908,7 +5804,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="I11" s="16" t="s">
         <v>33</v>
       </c>
@@ -5919,7 +5815,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="16.5" thickBot="1">
       <c r="I12" s="16" t="s">
         <v>38</v>
       </c>
@@ -5930,7 +5826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="91" t="s">
         <v>42</v>
       </c>
@@ -5949,7 +5845,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="16.5" thickBot="1">
       <c r="A14" s="26"/>
       <c r="B14" s="24"/>
       <c r="C14" s="24"/>
@@ -5966,7 +5862,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="23" t="s">
         <v>47</v>
       </c>
@@ -5984,7 +5880,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="67.25" customHeight="1">
       <c r="A16" s="26" t="s">
         <v>48</v>
       </c>
@@ -6008,7 +5904,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="32" customHeight="1" thickBot="1">
       <c r="A17" s="23" t="s">
         <v>45</v>
       </c>
@@ -6029,7 +5925,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="79.5" thickBot="1">
       <c r="A18" s="26" t="s">
         <v>49</v>
       </c>
@@ -6050,7 +5946,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="23" t="s">
         <v>11</v>
       </c>
@@ -6069,7 +5965,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="63.75" thickBot="1">
       <c r="A20" s="27" t="s">
         <v>52</v>
       </c>
@@ -6091,7 +5987,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="H21" s="16" t="str">
         <f>IF(INDEX(H4:H7,H20)=H4,"MA",IF(INDEX(H4:H7,H20)=H5,"CN",IF(INDEX(H4:H7,H20)=H6,"CS",IF(INDEX(H4:H7,H20)=H7,"LE"))))</f>
         <v>LE</v>
@@ -6108,122 +6004,122 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="K22" s="16">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="K23" s="16">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="K24" s="16">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="K25" s="16">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="K26" s="16">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="K27" s="16">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="K28" s="16">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="K29" s="16">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="K30" s="16">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="K31" s="16">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="K32" s="16">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="11:11">
       <c r="K33" s="16">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="11:11">
       <c r="K34" s="16">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="11:11">
       <c r="K35" s="16">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="11:11">
       <c r="K36" s="16">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="11:11">
       <c r="K37" s="16">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="11:11">
       <c r="K38" s="16">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="11:11">
       <c r="K39" s="16">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="11:11">
       <c r="K40" s="16">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="11:11">
       <c r="K41" s="16">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="11:11">
       <c r="K42" s="16">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="11:11">
       <c r="K43" s="16">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="11:11">
       <c r="K44" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="11:11">
       <c r="K45" s="16" t="str">
         <f>CONCATENATE("REC",K44,0)</f>
         <v>REC10</v>
@@ -6242,169 +6138,181 @@
     <mergeCell ref="D7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x14">
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1030" r:id="rId4" name="Drop Down 6">
+            <control shapeId="1030" r:id="rId3" name="Drop Down 6">
               <controlPr defaultSize="0" autoLine="0" autoPict="0" macro="[0]!Listadesplegable2_Cambiar">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>485775</xdr:rowOff>
+                    <xdr:rowOff>482600</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1019175</xdr:colOff>
+                    <xdr:colOff>1016000</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>714375</xdr:rowOff>
+                    <xdr:rowOff>711200</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1031" r:id="rId5" name="Drop Down 7">
+            <control shapeId="1031" r:id="rId4" name="Drop Down 7">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1019175</xdr:colOff>
+                    <xdr:colOff>1016000</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>485775</xdr:rowOff>
+                    <xdr:rowOff>482600</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>828675</xdr:colOff>
+                    <xdr:colOff>825500</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>714375</xdr:rowOff>
+                    <xdr:rowOff>711200</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1032" r:id="rId6" name="Drop Down 8">
+            <control shapeId="1032" r:id="rId5" name="Drop Down 8">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>485775</xdr:rowOff>
+                    <xdr:rowOff>482600</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>838200</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>714375</xdr:rowOff>
+                    <xdr:rowOff>711200</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1035" r:id="rId7" name="Drop Down 11">
+            <control shapeId="1035" r:id="rId6" name="Drop Down 11">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>485775</xdr:rowOff>
+                    <xdr:rowOff>482600</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>838200</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>714375</xdr:rowOff>
+                    <xdr:rowOff>711200</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1026" r:id="rId8" name="Drop Down 2">
+            <control shapeId="1026" r:id="rId7" name="Drop Down 2">
               <controlPr defaultSize="0" autoLine="0" autoPict="0" macro="[0]!Listadesplegable2_Cambiar">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>19050</xdr:colOff>
+                    <xdr:colOff>25400</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1038225</xdr:colOff>
+                    <xdr:colOff>1041400</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>238125</xdr:rowOff>
+                    <xdr:rowOff>241300</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1028" r:id="rId9" name="Drop Down 4">
+            <control shapeId="1028" r:id="rId8" name="Drop Down 4">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1047750</xdr:colOff>
+                    <xdr:colOff>1054100</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>866775</xdr:colOff>
+                    <xdr:colOff>863600</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>238125</xdr:rowOff>
+                    <xdr:rowOff>241300</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1029" r:id="rId10" name="Drop Down 5">
+            <control shapeId="1029" r:id="rId9" name="Drop Down 5">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>19050</xdr:colOff>
+                    <xdr:colOff>25400</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>238125</xdr:rowOff>
+                    <xdr:rowOff>241300</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
       </controls>
     </mc:Choice>
+    <mc:Fallback/>
   </mc:AlternateContent>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6417,22 +6325,22 @@
       <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21" style="16" customWidth="1"/>
-    <col min="2" max="2" width="22.25" style="16" customWidth="1"/>
-    <col min="3" max="3" width="17.375" style="16" customWidth="1"/>
-    <col min="4" max="4" width="10.875" style="16"/>
-    <col min="5" max="5" width="11.75" style="16" customWidth="1"/>
-    <col min="6" max="6" width="12.75" style="16" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" style="16" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="16"/>
+    <col min="5" max="5" width="11.6640625" style="16" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="16" customWidth="1"/>
     <col min="7" max="7" width="11" style="16" customWidth="1"/>
-    <col min="8" max="9" width="22.25" style="16" customWidth="1"/>
-    <col min="10" max="10" width="20.75" style="16" customWidth="1"/>
+    <col min="8" max="9" width="22.1640625" style="16" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" style="16" customWidth="1"/>
     <col min="11" max="11" width="44.5" style="16" customWidth="1"/>
-    <col min="12" max="16384" width="10.875" style="16"/>
+    <col min="12" max="16384" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="105" t="s">
         <v>57</v>
       </c>
@@ -6460,7 +6368,7 @@
       <c r="I1" s="106"/>
       <c r="J1" s="106"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="105"/>
       <c r="B2" s="105"/>
       <c r="C2" s="105"/>
@@ -6478,7 +6386,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="32" customFormat="1">
       <c r="A3" s="31" t="s">
         <v>70</v>
       </c>
@@ -6502,7 +6410,7 @@
       <c r="I3" s="31"/>
       <c r="J3" s="31"/>
     </row>
-    <row r="4" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="32" customFormat="1">
       <c r="A4" s="33" t="s">
         <v>58</v>
       </c>
@@ -6530,7 +6438,7 @@
       </c>
       <c r="J4" s="33"/>
     </row>
-    <row r="5" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="32" customFormat="1">
       <c r="A5" s="34" t="s">
         <v>81</v>
       </c>
@@ -6558,7 +6466,7 @@
       </c>
       <c r="J5" s="35"/>
     </row>
-    <row r="6" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="32" customFormat="1">
       <c r="A6" s="33" t="s">
         <v>59</v>
       </c>
@@ -6590,7 +6498,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="32" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="32" customFormat="1" ht="25.5">
       <c r="A7" s="33" t="s">
         <v>85</v>
       </c>
@@ -6618,7 +6526,7 @@
       </c>
       <c r="J7" s="33"/>
     </row>
-    <row r="8" spans="1:11" s="32" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="32" customFormat="1" ht="25.5">
       <c r="A8" s="33" t="s">
         <v>87</v>
       </c>
@@ -6646,7 +6554,7 @@
       </c>
       <c r="J8" s="33"/>
     </row>
-    <row r="9" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="32" customFormat="1">
       <c r="A9" s="33" t="s">
         <v>89</v>
       </c>
@@ -6674,7 +6582,7 @@
       </c>
       <c r="J9" s="33"/>
     </row>
-    <row r="10" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="32" customFormat="1">
       <c r="A10" s="33" t="s">
         <v>91</v>
       </c>
@@ -6698,7 +6606,7 @@
       <c r="I10" s="33"/>
       <c r="J10" s="33"/>
     </row>
-    <row r="11" spans="1:11" s="32" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="32" customFormat="1" ht="25.5">
       <c r="A11" s="33" t="s">
         <v>94</v>
       </c>
@@ -6726,7 +6634,7 @@
       </c>
       <c r="J11" s="33"/>
     </row>
-    <row r="12" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="32" customFormat="1">
       <c r="A12" s="33" t="s">
         <v>96</v>
       </c>
@@ -6754,7 +6662,7 @@
       </c>
       <c r="J12" s="33"/>
     </row>
-    <row r="13" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="63">
       <c r="A13" s="36" t="s">
         <v>98</v>
       </c>
@@ -6781,7 +6689,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="36" t="s">
         <v>102</v>
       </c>
@@ -6805,7 +6713,7 @@
       </c>
       <c r="J14" s="36"/>
     </row>
-    <row r="15" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="31.5">
       <c r="A15" s="36" t="s">
         <v>104</v>
       </c>
@@ -6832,7 +6740,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="94.5">
       <c r="A16" s="38" t="s">
         <v>108</v>
       </c>
@@ -6861,7 +6769,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="25.5">
       <c r="A17" s="33" t="s">
         <v>113</v>
       </c>
@@ -6890,12 +6798,12 @@
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="42" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="43" t="s">
         <v>120</v>
       </c>
@@ -6908,7 +6816,7 @@
       <c r="D21" s="44"/>
       <c r="E21" s="44"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="46" t="s">
         <v>123</v>
       </c>
@@ -6921,7 +6829,7 @@
       <c r="D22" s="47"/>
       <c r="E22" s="47"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="46" t="s">
         <v>126</v>
       </c>
@@ -6934,7 +6842,7 @@
       <c r="D23" s="47"/>
       <c r="E23" s="47"/>
     </row>
-    <row r="24" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="31.5">
       <c r="A24" s="46" t="s">
         <v>129</v>
       </c>
@@ -6947,7 +6855,7 @@
       <c r="D24" s="47"/>
       <c r="E24" s="47"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="46" t="s">
         <v>132</v>
       </c>
@@ -6960,7 +6868,7 @@
       <c r="D25" s="47"/>
       <c r="E25" s="47"/>
     </row>
-    <row r="26" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="63">
       <c r="A26" s="46" t="s">
         <v>135</v>
       </c>
@@ -6985,6 +6893,10 @@
     <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>